<commit_message>
Completed Advanced U Automation task which demo multiple scopes, moving data between app and excel.
</commit_message>
<xml_diff>
--- a/DemoExcel/Demo Excel.xlsx
+++ b/DemoExcel/Demo Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnetteKniberg\Documents\UiPath\UIPath_CertificationCourse_AdvancedRPA\UI Automation\DemoExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6FF665A-44A5-40BA-9173-5DA4C8F9F99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7F84E5-57BA-47C1-9D01-F82064CF4DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{812EB52E-482B-4EBD-8ADC-76005DA71907}"/>
+    <workbookView xWindow="3825" yWindow="6675" windowWidth="21600" windowHeight="8955" xr2:uid="{812EB52E-482B-4EBD-8ADC-76005DA71907}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,14 +414,14 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -449,6 +449,9 @@
       <c r="C2">
         <v>400</v>
       </c>
+      <c r="D2">
+        <v>247181</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -460,6 +463,9 @@
       <c r="C3">
         <v>100</v>
       </c>
+      <c r="D3">
+        <v>247182</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -471,6 +477,9 @@
       <c r="C4">
         <v>50</v>
       </c>
+      <c r="D4">
+        <v>247183</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -482,6 +491,9 @@
       <c r="C5">
         <v>599</v>
       </c>
+      <c r="D5">
+        <v>247184</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -492,6 +504,9 @@
       </c>
       <c r="C6">
         <v>599</v>
+      </c>
+      <c r="D6">
+        <v>247185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>